<commit_message>
mise a jour des taches effectues dans le fichier estimation.xlsx
Ajout des taches effectues dans le fichier excel.
</commit_message>
<xml_diff>
--- a/descriptionProjet/estimation.xlsx
+++ b/descriptionProjet/estimation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -151,6 +151,33 @@
   </si>
   <si>
     <t>gerer la lecture de la musique suit au mouvement du telephone</t>
+  </si>
+  <si>
+    <t>realisation de mon menu de slide</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>affichage des musique de mon telephone dans une activité</t>
+  </si>
+  <si>
+    <t>la musique demarre suit à un click</t>
+  </si>
+  <si>
+    <t>realisation de l'interface principale de mon application, test de fonctionement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture sur le fonctionement d'un service </t>
+  </si>
+  <si>
+    <t>Test personnels sur le fonctionement d'un service et son utilisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controle de la lecture de la musique( l'utilisateur peut aller a la musique suivante, precedente,) </t>
   </si>
 </sst>
 </file>
@@ -294,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -349,6 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1605,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1787,7 +1815,7 @@
         <v>40</v>
       </c>
       <c r="C29" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1797,7 +1825,9 @@
       <c r="B30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
@@ -1851,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1909,39 +1939,81 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12">
+        <v>42765</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="12">
+        <v>42765</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="12">
+        <v>42766</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="12">
+        <v>42766</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="24">
+        <v>42772</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
+      <c r="A19" s="24">
+        <v>42773</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
+      <c r="A20" s="24">
+        <v>42778</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
@@ -2085,7 +2157,7 @@
   <dimension ref="A6:C47"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD47"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
premiere remise du projet
Il est fonctionnel !!!!!!!!!
</commit_message>
<xml_diff>
--- a/descriptionProjet/estimation.xlsx
+++ b/descriptionProjet/estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -156,12 +156,6 @@
     <t>realisation de mon menu de slide</t>
   </si>
   <si>
-    <t>3h</t>
-  </si>
-  <si>
-    <t>2h</t>
-  </si>
-  <si>
     <t>affichage des musique de mon telephone dans une activité</t>
   </si>
   <si>
@@ -178,6 +172,9 @@
   </si>
   <si>
     <t xml:space="preserve">Controle de la lecture de la musique( l'utilisateur peut aller a la musique suivante, precedente,) </t>
+  </si>
+  <si>
+    <t>Lecture de la musique sur deux activites</t>
   </si>
 </sst>
 </file>
@@ -321,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,6 +358,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -376,7 +377,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1633,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1742,10 +1748,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="20"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="11">
         <f>SUM(C16:C20)</f>
         <v>50</v>
@@ -1851,10 +1857,10 @@
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="20"/>
+      <c r="B34" s="22"/>
       <c r="C34" s="11">
         <f>SUM(C26:C33)</f>
         <v>40</v>
@@ -1881,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1939,89 +1945,91 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
+      <c r="A14" s="26">
         <v>42765</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="27"/>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="26">
+        <v>42766</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="12">
-        <v>42765</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="C16" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="27"/>
+      <c r="B17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="20">
+        <v>42772</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="19">
+        <v>42773</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="19">
+        <v>42778</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="12">
-        <v>42766</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="12">
-        <v>42766</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="24">
-        <v>42772</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="24">
-        <v>42773</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="24">
-        <v>42778</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="19">
+        <v>42779</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
+      <c r="C21" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
@@ -2096,13 +2104,13 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2124,27 +2132,29 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="23"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="22"/>
+      <c r="B43" s="24"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
+      <c r="B44" s="24"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="22"/>
+      <c r="B45" s="24"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="22"/>
+      <c r="B46" s="24"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="23"/>
+      <c r="B47" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="B42:B47"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2156,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2214,7 +2224,9 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="12">
+        <v>42786</v>
+      </c>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
@@ -2331,10 +2343,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2359,22 +2371,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="23"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="22"/>
+      <c r="B43" s="24"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
+      <c r="B44" s="24"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="22"/>
+      <c r="B45" s="24"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="22"/>
+      <c r="B46" s="24"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="23"/>
+      <c r="B47" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2564,10 +2576,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2592,22 +2604,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="23"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="22"/>
+      <c r="B43" s="24"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
+      <c r="B44" s="24"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="22"/>
+      <c r="B45" s="24"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="22"/>
+      <c r="B46" s="24"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="23"/>
+      <c r="B47" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2797,10 +2809,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2825,22 +2837,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="23"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="22"/>
+      <c r="B43" s="24"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
+      <c r="B44" s="24"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="22"/>
+      <c r="B45" s="24"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="22"/>
+      <c r="B46" s="24"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="23"/>
+      <c r="B47" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Menu Favoris intégré et fonctionnel. Fonctionnalité theme en cour.
Je peux ajouter des musiques a mon menu de favoris. Aussi j'ai commence
le changement de mes themes.
</commit_message>
<xml_diff>
--- a/descriptionProjet/estimation.xlsx
+++ b/descriptionProjet/estimation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Semaine 15</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Le projet doit être décomposé en plusieurs sections indépendantes qui doivent être priorisées et estimées</t>
   </si>
   <si>
@@ -175,6 +172,33 @@
   </si>
   <si>
     <t>Lecture de la musique sur deux activites</t>
+  </si>
+  <si>
+    <t>Mise en place de mon propre controlleur</t>
+  </si>
+  <si>
+    <t>Faire une seconde activité dediée au control de la musique. La rendre fonctionnelle, faire fonctionner la seekBar</t>
+  </si>
+  <si>
+    <t>Ajout des fonctionnalites a mon propre controlleur(next, previous, pause, lecture)</t>
+  </si>
+  <si>
+    <t>Faire fonctionner la lecture aleatoire</t>
+  </si>
+  <si>
+    <t>acces a mon activité favoris(probleme avec le manifest) et correction de quelques bugs decouverts</t>
+  </si>
+  <si>
+    <t>creation de ma BD sqlite pour garder les informations sur les musiques du menu favoris, test de l'ajout des musiques dans le menu favoris via l'activité controlleur (icone en coeur)</t>
+  </si>
+  <si>
+    <t>Mise en place de l'activité favoris. Afficher les musiques favoris ajoutés dans la BDSQLite. Faire lire la bonne liste de musique en fonction de l'activité dans la quelle on a lance la musique( En gros, la gestion de la bibliotheque et des favoris simultanement)</t>
+  </si>
+  <si>
+    <t>faire l'interface de l'activité des themes, modifier la couleur de background de mes activités en fonction du theme choisit.</t>
+  </si>
+  <si>
+    <t>Bug découvert. Quand la musique de la bibliotheque joue et que je vais dans l'activité favoris</t>
   </si>
 </sst>
 </file>
@@ -318,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -362,6 +386,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -382,6 +418,18 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,16 +574,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3710940</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -559,8 +607,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4229100" y="0"/>
-          <a:ext cx="1790700" cy="678180"/>
+          <a:off x="5021580" y="68580"/>
+          <a:ext cx="1303020" cy="678180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1639,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C36"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1652,7 +1700,7 @@
   <sheetData>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1697,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="3">
         <v>10</v>
@@ -1708,7 +1756,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="3">
         <v>10</v>
@@ -1719,7 +1767,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3">
         <v>15</v>
@@ -1730,7 +1778,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="3">
         <v>5</v>
@@ -1741,17 +1789,17 @@
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="22"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="11">
         <f>SUM(C16:C20)</f>
         <v>50</v>
@@ -1785,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="3">
         <v>15</v>
@@ -1796,7 +1844,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="3">
         <v>5</v>
@@ -1807,7 +1855,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="3">
         <v>10</v>
@@ -1818,7 +1866,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="3">
         <v>5</v>
@@ -1829,7 +1877,7 @@
         <v>5</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="3">
         <v>5</v>
@@ -1857,10 +1905,10 @@
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="22"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="11">
         <f>SUM(C26:C33)</f>
         <v>40</v>
@@ -1887,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView view="pageLayout" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1945,51 +1993,51 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="26">
+      <c r="A14" s="30">
         <v>42765</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>44</v>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C14" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="4" t="s">
-        <v>47</v>
+      <c r="A15" s="31"/>
+      <c r="B15" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C15" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="26">
+      <c r="A16" s="30">
         <v>42766</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>45</v>
+      <c r="B16" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C16" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
-      <c r="B17" s="4" t="s">
-        <v>46</v>
+      <c r="A17" s="31"/>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C17" s="15">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <v>42772</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>50</v>
+      <c r="B18" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="C18" s="15">
         <v>3</v>
@@ -1999,8 +2047,8 @@
       <c r="A19" s="19">
         <v>42773</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>48</v>
+      <c r="B19" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="C19" s="15">
         <v>2</v>
@@ -2010,8 +2058,8 @@
       <c r="A20" s="19">
         <v>42778</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>49</v>
+      <c r="B20" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C20" s="15">
         <v>3</v>
@@ -2021,8 +2069,8 @@
       <c r="A21" s="19">
         <v>42779</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>51</v>
+      <c r="B21" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C21" s="15">
         <v>3</v>
@@ -2104,10 +2152,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="22"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>22</v>
@@ -2115,39 +2163,41 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="B40" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="23"/>
+        <v>32</v>
+      </c>
+      <c r="B42" s="27"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="24"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="24"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="24"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="24"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="25"/>
+      <c r="B47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2166,8 +2216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2223,63 +2273,117 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42786</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="19">
+        <v>42787</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="19">
+        <v>42788</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="19">
+        <v>42798</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="19">
+        <v>42799</v>
+      </c>
+      <c r="B18" s="35"/>
+      <c r="C18" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="15"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="15"/>
+      <c r="A19" s="19">
+        <v>42800</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="20">
+        <v>42801</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="20">
+        <v>42803</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="22">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="24">
+        <v>42807</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="24">
+        <v>42808</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="22">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -2343,24 +2447,24 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="22"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2369,29 +2473,31 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="23"/>
+        <v>32</v>
+      </c>
+      <c r="B42" s="27"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="24"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="24"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="24"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="24"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="25"/>
+      <c r="B47" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="B42:B47"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2576,10 +2682,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="22"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2587,13 +2693,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2602,24 +2708,24 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="23"/>
+        <v>32</v>
+      </c>
+      <c r="B42" s="27"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="24"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="24"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="24"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="24"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="25"/>
+      <c r="B47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2673,7 +2779,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2809,10 +2915,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="22"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2820,13 +2926,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2835,24 +2941,24 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="23"/>
+        <v>32</v>
+      </c>
+      <c r="B42" s="27"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="24"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="24"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="24"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="24"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="25"/>
+      <c r="B47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Changement de theme fonctionnel
L'utilisateur peut changer le theme de l'application.
</commit_message>
<xml_diff>
--- a/descriptionProjet/estimation.xlsx
+++ b/descriptionProjet/estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>faire l'interface de l'activité des themes, modifier la couleur de background de mes activités en fonction du theme choisit.</t>
+  </si>
+  <si>
+    <t>ajout d'une nouvelle table dans ma BD SqLite pour stocker mon theme, reglage de bug</t>
+  </si>
+  <si>
+    <t>réglage du bug lors de la creation de mes tables dans SQLLite</t>
+  </si>
+  <si>
+    <t>ajout d'un scrool view dans l'activite des themes (journée des présentations)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tests sur le fonctionnement de la sauvegarde du theme actif</t>
   </si>
 </sst>
 </file>
@@ -2213,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView view="pageLayout" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2377,17 +2389,21 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="15"/>
+      <c r="A24" s="19">
+        <v>42814</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
@@ -2448,7 +2464,7 @@
       <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2504,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD47"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2561,20 +2577,38 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="19">
+        <v>42821</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="19">
+        <v>42822</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="19">
+        <v>42828</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="15">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
@@ -2683,7 +2717,7 @@
       <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
menu dans les items du listView des favoris fonctionnel
j'ai integre un menu dans chaque items du listView de l,activité favoris
</commit_message>
<xml_diff>
--- a/descriptionProjet/estimation.xlsx
+++ b/descriptionProjet/estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Tests sur le fonctionnement de la sauvegarde du theme actif</t>
+  </si>
+  <si>
+    <t>WAQ à Québec</t>
+  </si>
+  <si>
+    <t>ajout de quelques images dans mon application, recherches sur le menu a mettre sur chaque items de mes listviews</t>
+  </si>
+  <si>
+    <t>test sur l'ajout de mon menu a chaque items de mes listviews dans l'activité Favoris</t>
   </si>
 </sst>
 </file>
@@ -351,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -439,6 +448,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2225,7 +2240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -2520,8 +2535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2611,9 +2626,15 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="19">
+        <v>42829</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
@@ -2717,7 +2738,7 @@
       <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2771,8 +2792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2828,20 +2849,36 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>42835</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="19">
+        <v>42836</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="19">
+        <v>42836</v>
+      </c>
+      <c r="B16" s="37"/>
+      <c r="C16" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
@@ -2950,7 +2987,7 @@
       <c r="B37" s="26"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2990,9 +3027,10 @@
       <c r="B47" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="B42:B47"/>
+    <mergeCell ref="B15:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>